<commit_message>
Added temp basal events structure to docu
</commit_message>
<xml_diff>
--- a/doc/Bayer-Medtronic-640G USB HID Interface.xlsx
+++ b/doc/Bayer-Medtronic-640G USB HID Interface.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Projects\pump_data_downloader\decoding_contour_next_link\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Projects\pump_data_downloader\decoding_contour_next_link\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,8 +36,48 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Pawel Kowalik</author>
+  </authors>
+  <commentList>
+    <comment ref="N9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0-8
+0 - no preset</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0 - fixed rate
+1 - percent rate</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="261">
   <si>
     <t>Byte</t>
   </si>
@@ -785,12 +825,48 @@
   <si>
     <t>Contained by: MULTIPACKET_SEGMENT_TRANSMISSION as response to READ_HISTORY_REQUEST 0x0304</t>
   </si>
+  <si>
+    <t>TEMP_BASAL_PROGRAMMED</t>
+  </si>
+  <si>
+    <t>0x1B</t>
+  </si>
+  <si>
+    <t>TEMP_BASAL_COMPLETE</t>
+  </si>
+  <si>
+    <t>0x22</t>
+  </si>
+  <si>
+    <t>0801000000009605a0</t>
+  </si>
+  <si>
+    <t>0801000000009605a0010001</t>
+  </si>
+  <si>
+    <t>presetID</t>
+  </si>
+  <si>
+    <t>tempBasalType</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>time (min)</t>
+  </si>
+  <si>
+    <t>basal rate * 10000</t>
+  </si>
+  <si>
+    <t>real time (min)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -866,8 +942,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -934,6 +1025,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -953,7 +1050,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1050,6 +1147,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1068,11 +1169,13 @@
     <xf numFmtId="49" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1081,12 +1184,13 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1419,68 +1523,68 @@
       </c>
     </row>
     <row r="2" spans="2:66" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42"/>
-      <c r="W2" s="42"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="42"/>
-      <c r="Z2" s="42"/>
-      <c r="AA2" s="42"/>
-      <c r="AB2" s="42"/>
-      <c r="AC2" s="42"/>
-      <c r="AD2" s="42"/>
-      <c r="AE2" s="42"/>
-      <c r="AF2" s="42"/>
-      <c r="AG2" s="42"/>
-      <c r="AH2" s="42"/>
-      <c r="AI2" s="42"/>
-      <c r="AJ2" s="42"/>
-      <c r="AK2" s="42"/>
-      <c r="AL2" s="42"/>
-      <c r="AM2" s="42"/>
-      <c r="AN2" s="42"/>
-      <c r="AO2" s="42"/>
-      <c r="AP2" s="42"/>
-      <c r="AQ2" s="42"/>
-      <c r="AR2" s="42"/>
-      <c r="AS2" s="42"/>
-      <c r="AT2" s="42"/>
-      <c r="AU2" s="42"/>
-      <c r="AV2" s="42"/>
-      <c r="AW2" s="42"/>
-      <c r="AX2" s="42"/>
-      <c r="AY2" s="42"/>
-      <c r="AZ2" s="42"/>
-      <c r="BA2" s="42"/>
-      <c r="BB2" s="42"/>
-      <c r="BC2" s="42"/>
-      <c r="BD2" s="42"/>
-      <c r="BE2" s="42"/>
-      <c r="BF2" s="42"/>
-      <c r="BG2" s="42"/>
-      <c r="BH2" s="42"/>
-      <c r="BI2" s="42"/>
-      <c r="BJ2" s="42"/>
-      <c r="BK2" s="42"/>
-      <c r="BL2" s="42"/>
-      <c r="BM2" s="42"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
+      <c r="V2" s="46"/>
+      <c r="W2" s="46"/>
+      <c r="X2" s="46"/>
+      <c r="Y2" s="46"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
+      <c r="AF2" s="46"/>
+      <c r="AG2" s="46"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="46"/>
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="46"/>
+      <c r="AT2" s="46"/>
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="46"/>
+      <c r="AW2" s="46"/>
+      <c r="AX2" s="46"/>
+      <c r="AY2" s="46"/>
+      <c r="AZ2" s="46"/>
+      <c r="BA2" s="46"/>
+      <c r="BB2" s="46"/>
+      <c r="BC2" s="46"/>
+      <c r="BD2" s="46"/>
+      <c r="BE2" s="46"/>
+      <c r="BF2" s="46"/>
+      <c r="BG2" s="46"/>
+      <c r="BH2" s="46"/>
+      <c r="BI2" s="46"/>
+      <c r="BJ2" s="46"/>
+      <c r="BK2" s="46"/>
+      <c r="BL2" s="46"/>
+      <c r="BM2" s="46"/>
     </row>
     <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1695,68 +1799,68 @@
       <c r="F4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
-      <c r="AC4" s="43"/>
-      <c r="AD4" s="43"/>
-      <c r="AE4" s="43"/>
-      <c r="AF4" s="43"/>
-      <c r="AG4" s="43"/>
-      <c r="AH4" s="43"/>
-      <c r="AI4" s="43"/>
-      <c r="AJ4" s="43"/>
-      <c r="AK4" s="43"/>
-      <c r="AL4" s="43"/>
-      <c r="AM4" s="43"/>
-      <c r="AN4" s="43"/>
-      <c r="AO4" s="43"/>
-      <c r="AP4" s="43"/>
-      <c r="AQ4" s="43"/>
-      <c r="AR4" s="43"/>
-      <c r="AS4" s="43"/>
-      <c r="AT4" s="43"/>
-      <c r="AU4" s="43"/>
-      <c r="AV4" s="43"/>
-      <c r="AW4" s="43"/>
-      <c r="AX4" s="43"/>
-      <c r="AY4" s="43"/>
-      <c r="AZ4" s="43"/>
-      <c r="BA4" s="43"/>
-      <c r="BB4" s="43"/>
-      <c r="BC4" s="43"/>
-      <c r="BD4" s="43"/>
-      <c r="BE4" s="43"/>
-      <c r="BF4" s="43"/>
-      <c r="BG4" s="43"/>
-      <c r="BH4" s="43"/>
-      <c r="BI4" s="43"/>
-      <c r="BJ4" s="43"/>
-      <c r="BK4" s="43"/>
-      <c r="BL4" s="43"/>
-      <c r="BM4" s="43"/>
-      <c r="BN4" s="43"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="47"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="47"/>
+      <c r="Y4" s="47"/>
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="47"/>
+      <c r="AC4" s="47"/>
+      <c r="AD4" s="47"/>
+      <c r="AE4" s="47"/>
+      <c r="AF4" s="47"/>
+      <c r="AG4" s="47"/>
+      <c r="AH4" s="47"/>
+      <c r="AI4" s="47"/>
+      <c r="AJ4" s="47"/>
+      <c r="AK4" s="47"/>
+      <c r="AL4" s="47"/>
+      <c r="AM4" s="47"/>
+      <c r="AN4" s="47"/>
+      <c r="AO4" s="47"/>
+      <c r="AP4" s="47"/>
+      <c r="AQ4" s="47"/>
+      <c r="AR4" s="47"/>
+      <c r="AS4" s="47"/>
+      <c r="AT4" s="47"/>
+      <c r="AU4" s="47"/>
+      <c r="AV4" s="47"/>
+      <c r="AW4" s="47"/>
+      <c r="AX4" s="47"/>
+      <c r="AY4" s="47"/>
+      <c r="AZ4" s="47"/>
+      <c r="BA4" s="47"/>
+      <c r="BB4" s="47"/>
+      <c r="BC4" s="47"/>
+      <c r="BD4" s="47"/>
+      <c r="BE4" s="47"/>
+      <c r="BF4" s="47"/>
+      <c r="BG4" s="47"/>
+      <c r="BH4" s="47"/>
+      <c r="BI4" s="47"/>
+      <c r="BJ4" s="47"/>
+      <c r="BK4" s="47"/>
+      <c r="BL4" s="47"/>
+      <c r="BM4" s="47"/>
+      <c r="BN4" s="47"/>
     </row>
     <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
@@ -2350,26 +2454,26 @@
       <c r="L7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="46" t="s">
+      <c r="M7" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46"/>
-      <c r="S7" s="46"/>
-      <c r="T7" s="46"/>
-      <c r="U7" s="45" t="s">
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="50"/>
+      <c r="U7" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="45"/>
-      <c r="AA7" s="45"/>
-      <c r="AB7" s="45"/>
+      <c r="V7" s="49"/>
+      <c r="W7" s="49"/>
+      <c r="X7" s="49"/>
+      <c r="Y7" s="49"/>
+      <c r="Z7" s="49"/>
+      <c r="AA7" s="49"/>
+      <c r="AB7" s="49"/>
       <c r="AC7" s="35"/>
       <c r="AD7" s="35"/>
       <c r="AE7" s="35"/>
@@ -3074,16 +3178,16 @@
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
       <c r="K7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3093,17 +3197,17 @@
       <c r="M7" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="47" t="s">
+      <c r="N7" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="47"/>
-      <c r="S7" s="47"/>
-      <c r="T7" s="47"/>
-      <c r="U7" s="47"/>
-      <c r="V7" s="47"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="51"/>
+      <c r="S7" s="51"/>
+      <c r="T7" s="51"/>
+      <c r="U7" s="51"/>
+      <c r="V7" s="51"/>
       <c r="W7" s="35"/>
       <c r="X7" s="35"/>
       <c r="Y7" s="35"/>
@@ -4414,26 +4518,26 @@
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="46" t="s">
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46"/>
-      <c r="S7" s="46"/>
-      <c r="T7" s="46"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="50"/>
       <c r="U7" s="35" t="s">
         <v>130</v>
       </c>
@@ -4446,22 +4550,22 @@
       <c r="X7" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="Y7" s="47" t="s">
+      <c r="Y7" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="Z7" s="47"/>
-      <c r="AA7" s="47"/>
-      <c r="AB7" s="47"/>
-      <c r="AC7" s="47"/>
-      <c r="AD7" s="47"/>
-      <c r="AE7" s="47"/>
-      <c r="AF7" s="47"/>
-      <c r="AG7" s="47"/>
-      <c r="AH7" s="47"/>
-      <c r="AI7" s="47"/>
-      <c r="AJ7" s="47"/>
-      <c r="AK7" s="47"/>
-      <c r="AL7" s="47"/>
+      <c r="Z7" s="51"/>
+      <c r="AA7" s="51"/>
+      <c r="AB7" s="51"/>
+      <c r="AC7" s="51"/>
+      <c r="AD7" s="51"/>
+      <c r="AE7" s="51"/>
+      <c r="AF7" s="51"/>
+      <c r="AG7" s="51"/>
+      <c r="AH7" s="51"/>
+      <c r="AI7" s="51"/>
+      <c r="AJ7" s="51"/>
+      <c r="AK7" s="51"/>
+      <c r="AL7" s="51"/>
       <c r="AM7" s="35"/>
       <c r="AN7" s="35"/>
       <c r="AO7" s="35"/>
@@ -4728,11 +4832,11 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7:T7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4866,215 +4970,215 @@
         <v>0</v>
       </c>
       <c r="C4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(C4)-COLUMN($C4),2)</f>
+        <f t="shared" ref="C4:AH4" si="0">"0x" &amp; DEC2HEX(COLUMN(C4)-COLUMN($C4),2)</f>
         <v>0x00</v>
       </c>
       <c r="D4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(D4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x01</v>
       </c>
       <c r="E4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(E4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x02</v>
       </c>
       <c r="F4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(F4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x03</v>
       </c>
       <c r="G4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(G4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x04</v>
       </c>
       <c r="H4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(H4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x05</v>
       </c>
       <c r="I4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(I4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x06</v>
       </c>
       <c r="J4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(J4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x07</v>
       </c>
       <c r="K4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(K4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x08</v>
       </c>
       <c r="L4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(L4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x09</v>
       </c>
       <c r="M4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(M4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x0A</v>
       </c>
       <c r="N4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(N4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x0B</v>
       </c>
       <c r="O4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(O4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x0C</v>
       </c>
       <c r="P4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(P4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x0D</v>
       </c>
       <c r="Q4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(Q4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x0E</v>
       </c>
       <c r="R4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(R4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x0F</v>
       </c>
       <c r="S4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(S4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x10</v>
       </c>
       <c r="T4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(T4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x11</v>
       </c>
       <c r="U4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(U4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x12</v>
       </c>
       <c r="V4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(V4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x13</v>
       </c>
       <c r="W4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(W4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x14</v>
       </c>
       <c r="X4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(X4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x15</v>
       </c>
       <c r="Y4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(Y4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x16</v>
       </c>
       <c r="Z4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(Z4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x17</v>
       </c>
       <c r="AA4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AA4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x18</v>
       </c>
       <c r="AB4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AB4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x19</v>
       </c>
       <c r="AC4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AC4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x1A</v>
       </c>
       <c r="AD4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AD4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x1B</v>
       </c>
       <c r="AE4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AE4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x1C</v>
       </c>
       <c r="AF4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AF4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x1D</v>
       </c>
       <c r="AG4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AG4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x1E</v>
       </c>
       <c r="AH4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AH4)-COLUMN($C4),2)</f>
+        <f t="shared" si="0"/>
         <v>0x1F</v>
       </c>
       <c r="AI4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AI4)-COLUMN($C4),2)</f>
+        <f t="shared" ref="AI4:BC4" si="1">"0x" &amp; DEC2HEX(COLUMN(AI4)-COLUMN($C4),2)</f>
         <v>0x20</v>
       </c>
       <c r="AJ4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AJ4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x21</v>
       </c>
       <c r="AK4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AK4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x22</v>
       </c>
       <c r="AL4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AL4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x23</v>
       </c>
       <c r="AM4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AM4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x24</v>
       </c>
       <c r="AN4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AN4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x25</v>
       </c>
       <c r="AO4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AO4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x26</v>
       </c>
       <c r="AP4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AP4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x27</v>
       </c>
       <c r="AQ4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AQ4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x28</v>
       </c>
       <c r="AR4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AR4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x29</v>
       </c>
       <c r="AS4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AS4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x2A</v>
       </c>
       <c r="AT4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AT4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x2B</v>
       </c>
       <c r="AU4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AU4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x2C</v>
       </c>
       <c r="AV4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AV4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x2D</v>
       </c>
       <c r="AW4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AW4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x2E</v>
       </c>
       <c r="AX4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AX4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x2F</v>
       </c>
       <c r="AY4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AY4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x30</v>
       </c>
       <c r="AZ4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(AZ4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x31</v>
       </c>
       <c r="BA4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(BA4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x32</v>
       </c>
       <c r="BB4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(BB4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x33</v>
       </c>
       <c r="BC4" s="6" t="str">
-        <f>"0x" &amp; DEC2HEX(COLUMN(BC4)-COLUMN($C4),2)</f>
+        <f t="shared" si="1"/>
         <v>0x34</v>
       </c>
     </row>
@@ -5088,41 +5192,41 @@
       <c r="D5" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="54" t="s">
         <v>245</v>
       </c>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="53"/>
-      <c r="T5" s="53"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
       <c r="U5" s="35"/>
       <c r="V5" s="35"/>
       <c r="W5" s="35"/>
       <c r="X5" s="35"/>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="54"/>
-      <c r="AC5" s="54"/>
-      <c r="AD5" s="54"/>
-      <c r="AE5" s="54"/>
-      <c r="AF5" s="54"/>
-      <c r="AG5" s="54"/>
-      <c r="AH5" s="54"/>
-      <c r="AI5" s="54"/>
-      <c r="AJ5" s="54"/>
-      <c r="AK5" s="54"/>
-      <c r="AL5" s="54"/>
+      <c r="Y5" s="44"/>
+      <c r="Z5" s="44"/>
+      <c r="AA5" s="44"/>
+      <c r="AB5" s="44"/>
+      <c r="AC5" s="44"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="44"/>
+      <c r="AF5" s="44"/>
+      <c r="AG5" s="44"/>
+      <c r="AH5" s="44"/>
+      <c r="AI5" s="44"/>
+      <c r="AJ5" s="44"/>
+      <c r="AK5" s="44"/>
+      <c r="AL5" s="44"/>
       <c r="AM5" s="17"/>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
@@ -5132,68 +5236,68 @@
       <c r="C6" t="s">
         <v>243</v>
       </c>
-      <c r="N6" s="53" t="s">
+      <c r="N6" s="43" t="s">
         <v>239</v>
       </c>
-      <c r="O6" s="53" t="s">
+      <c r="O6" s="43" t="s">
         <v>238</v>
       </c>
-      <c r="P6" s="53" t="s">
+      <c r="P6" s="43" t="s">
         <v>237</v>
       </c>
-      <c r="Q6" s="52" t="s">
+      <c r="Q6" s="56" t="s">
         <v>236</v>
       </c>
-      <c r="R6" s="52"/>
-      <c r="S6" s="52"/>
-      <c r="T6" s="52"/>
-      <c r="U6" s="49" t="s">
+      <c r="R6" s="56"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="56"/>
+      <c r="U6" s="53" t="s">
         <v>242</v>
       </c>
-      <c r="V6" s="49"/>
-      <c r="W6" s="49"/>
-      <c r="X6" s="49"/>
-      <c r="Y6" s="52" t="s">
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
+      <c r="X6" s="53"/>
+      <c r="Y6" s="56" t="s">
         <v>223</v>
       </c>
-      <c r="Z6" s="52"/>
-      <c r="AA6" s="52"/>
-      <c r="AB6" s="52"/>
+      <c r="Z6" s="56"/>
+      <c r="AA6" s="56"/>
+      <c r="AB6" s="56"/>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>241</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="42" t="s">
         <v>240</v>
       </c>
-      <c r="N7" s="53" t="s">
+      <c r="N7" s="43" t="s">
         <v>239</v>
       </c>
-      <c r="O7" s="53" t="s">
+      <c r="O7" s="43" t="s">
         <v>238</v>
       </c>
-      <c r="P7" s="53" t="s">
+      <c r="P7" s="43" t="s">
         <v>237</v>
       </c>
-      <c r="Q7" s="52" t="s">
+      <c r="Q7" s="56" t="s">
         <v>236</v>
       </c>
-      <c r="R7" s="52"/>
-      <c r="S7" s="52"/>
-      <c r="T7" s="52"/>
-      <c r="U7" s="49" t="s">
+      <c r="R7" s="56"/>
+      <c r="S7" s="56"/>
+      <c r="T7" s="56"/>
+      <c r="U7" s="53" t="s">
         <v>223</v>
       </c>
-      <c r="V7" s="49"/>
-      <c r="W7" s="49"/>
-      <c r="X7" s="49"/>
+      <c r="V7" s="53"/>
+      <c r="W7" s="53"/>
+      <c r="X7" s="53"/>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>235</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="42" t="s">
         <v>234</v>
       </c>
       <c r="N8" s="3" t="s">
@@ -5202,91 +5306,168 @@
       <c r="O8" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="P8" s="51" t="s">
+      <c r="P8" s="55" t="s">
         <v>231</v>
       </c>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="49" t="s">
+      <c r="Q8" s="55"/>
+      <c r="R8" s="53" t="s">
         <v>230</v>
       </c>
-      <c r="S8" s="49"/>
-      <c r="T8" s="50" t="s">
+      <c r="S8" s="53"/>
+      <c r="T8" s="52" t="s">
         <v>229</v>
       </c>
-      <c r="U8" s="50"/>
-      <c r="V8" s="49" t="s">
+      <c r="U8" s="52"/>
+      <c r="V8" s="53" t="s">
         <v>228</v>
       </c>
-      <c r="W8" s="49"/>
-      <c r="X8" s="49"/>
-      <c r="Y8" s="49"/>
-      <c r="Z8" s="50" t="s">
+      <c r="W8" s="53"/>
+      <c r="X8" s="53"/>
+      <c r="Y8" s="53"/>
+      <c r="Z8" s="52" t="s">
         <v>227</v>
       </c>
-      <c r="AA8" s="50"/>
-      <c r="AB8" s="49" t="s">
+      <c r="AA8" s="52"/>
+      <c r="AB8" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="AC8" s="49"/>
-      <c r="AD8" s="50" t="s">
+      <c r="AC8" s="53"/>
+      <c r="AD8" s="52" t="s">
         <v>225</v>
       </c>
-      <c r="AE8" s="50"/>
-      <c r="AF8" s="50"/>
-      <c r="AG8" s="50"/>
-      <c r="AH8" s="49" t="s">
+      <c r="AE8" s="52"/>
+      <c r="AF8" s="52"/>
+      <c r="AG8" s="52"/>
+      <c r="AH8" s="53" t="s">
         <v>224</v>
       </c>
-      <c r="AI8" s="49"/>
-      <c r="AJ8" s="49"/>
-      <c r="AK8" s="49"/>
-      <c r="AL8" s="50" t="s">
+      <c r="AI8" s="53"/>
+      <c r="AJ8" s="53"/>
+      <c r="AK8" s="53"/>
+      <c r="AL8" s="52" t="s">
         <v>223</v>
       </c>
-      <c r="AM8" s="50"/>
-      <c r="AN8" s="50"/>
-      <c r="AO8" s="50"/>
-      <c r="AP8" s="49" t="s">
+      <c r="AM8" s="52"/>
+      <c r="AN8" s="52"/>
+      <c r="AO8" s="52"/>
+      <c r="AP8" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="AQ8" s="49"/>
-      <c r="AR8" s="49"/>
-      <c r="AS8" s="49"/>
-      <c r="AT8" s="50" t="s">
+      <c r="AQ8" s="53"/>
+      <c r="AR8" s="53"/>
+      <c r="AS8" s="53"/>
+      <c r="AT8" s="52" t="s">
         <v>221</v>
       </c>
-      <c r="AU8" s="50"/>
-      <c r="AV8" s="50"/>
-      <c r="AW8" s="50"/>
+      <c r="AU8" s="52"/>
+      <c r="AV8" s="52"/>
+      <c r="AW8" s="52"/>
       <c r="AX8" s="3" t="s">
         <v>220</v>
       </c>
       <c r="AY8" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="AZ8" s="49" t="s">
+      <c r="AZ8" s="53" t="s">
         <v>218</v>
       </c>
-      <c r="BA8" s="49"/>
-      <c r="BB8" s="49"/>
-      <c r="BC8" s="49"/>
+      <c r="BA8" s="53"/>
+      <c r="BB8" s="53"/>
+      <c r="BC8" s="53"/>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="C9" s="48"/>
-      <c r="N9" s="48"/>
+      <c r="A9" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="N9" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="O9" s="59" t="s">
+        <v>256</v>
+      </c>
+      <c r="P9" s="60" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="60"/>
+      <c r="S9" s="60"/>
+      <c r="T9" s="58" t="s">
+        <v>257</v>
+      </c>
+      <c r="U9" s="60" t="s">
+        <v>258</v>
+      </c>
+      <c r="V9" s="60"/>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C10" t="s">
+        <v>252</v>
+      </c>
+      <c r="N10" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="O10" s="59" t="s">
+        <v>256</v>
+      </c>
+      <c r="P10" s="60" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q10" s="60"/>
+      <c r="R10" s="60"/>
+      <c r="S10" s="60"/>
+      <c r="T10" s="58" t="s">
+        <v>257</v>
+      </c>
+      <c r="U10" s="60" t="s">
+        <v>258</v>
+      </c>
+      <c r="V10" s="60"/>
+      <c r="W10" s="61" t="str">
+        <f t="shared" ref="W10" si="2">"0x"&amp;MID($B10,1+(COLUMN(W10)-COLUMN($N10))*2,2)</f>
+        <v>0x01</v>
+      </c>
+      <c r="X10" s="60" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y10" s="60"/>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="E16" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="AL8:AO8"/>
-    <mergeCell ref="AP8:AS8"/>
-    <mergeCell ref="AT8:AW8"/>
-    <mergeCell ref="AZ8:BC8"/>
-    <mergeCell ref="AH8:AK8"/>
-    <mergeCell ref="F5:M5"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="V8:Y8"/>
-    <mergeCell ref="T8:U8"/>
+  <mergeCells count="23">
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="X10:Y10"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="U10:V10"/>
     <mergeCell ref="AD8:AG8"/>
     <mergeCell ref="Z8:AA8"/>
     <mergeCell ref="AB8:AC8"/>
@@ -5295,9 +5476,20 @@
     <mergeCell ref="Y6:AB6"/>
     <mergeCell ref="U7:X7"/>
     <mergeCell ref="Q7:T7"/>
+    <mergeCell ref="F5:M5"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="V8:Y8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="AP8:AS8"/>
+    <mergeCell ref="AT8:AW8"/>
+    <mergeCell ref="AZ8:BC8"/>
+    <mergeCell ref="AH8:AK8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6759,33 +6951,33 @@
       <c r="AI5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AJ5" s="43" t="s">
+      <c r="AJ5" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="AK5" s="43"/>
-      <c r="AL5" s="43"/>
-      <c r="AM5" s="43"/>
-      <c r="AN5" s="43"/>
-      <c r="AO5" s="43"/>
-      <c r="AP5" s="43"/>
-      <c r="AQ5" s="43"/>
-      <c r="AR5" s="43"/>
-      <c r="AS5" s="43"/>
-      <c r="AT5" s="43"/>
-      <c r="AU5" s="43"/>
-      <c r="AV5" s="43"/>
-      <c r="AW5" s="43"/>
-      <c r="AX5" s="43"/>
-      <c r="AY5" s="43"/>
-      <c r="AZ5" s="43"/>
-      <c r="BA5" s="43"/>
-      <c r="BB5" s="43"/>
-      <c r="BC5" s="43"/>
-      <c r="BD5" s="43"/>
-      <c r="BE5" s="43"/>
-      <c r="BF5" s="43"/>
-      <c r="BG5" s="43"/>
-      <c r="BH5" s="43"/>
+      <c r="AK5" s="47"/>
+      <c r="AL5" s="47"/>
+      <c r="AM5" s="47"/>
+      <c r="AN5" s="47"/>
+      <c r="AO5" s="47"/>
+      <c r="AP5" s="47"/>
+      <c r="AQ5" s="47"/>
+      <c r="AR5" s="47"/>
+      <c r="AS5" s="47"/>
+      <c r="AT5" s="47"/>
+      <c r="AU5" s="47"/>
+      <c r="AV5" s="47"/>
+      <c r="AW5" s="47"/>
+      <c r="AX5" s="47"/>
+      <c r="AY5" s="47"/>
+      <c r="AZ5" s="47"/>
+      <c r="BA5" s="47"/>
+      <c r="BB5" s="47"/>
+      <c r="BC5" s="47"/>
+      <c r="BD5" s="47"/>
+      <c r="BE5" s="47"/>
+      <c r="BF5" s="47"/>
+      <c r="BG5" s="47"/>
+      <c r="BH5" s="47"/>
       <c r="BI5"/>
       <c r="BJ5"/>
       <c r="BK5"/>
@@ -7604,66 +7796,66 @@
       <c r="D5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="43"/>
-      <c r="Y5" s="43"/>
-      <c r="Z5" s="43"/>
-      <c r="AA5" s="43"/>
-      <c r="AB5" s="43"/>
-      <c r="AC5" s="43"/>
-      <c r="AD5" s="43"/>
-      <c r="AE5" s="43"/>
-      <c r="AF5" s="43"/>
-      <c r="AG5" s="43"/>
-      <c r="AH5" s="43"/>
-      <c r="AI5" s="43"/>
-      <c r="AJ5" s="43"/>
-      <c r="AK5" s="43"/>
-      <c r="AL5" s="43"/>
-      <c r="AM5" s="43"/>
-      <c r="AN5" s="43"/>
-      <c r="AO5" s="43"/>
-      <c r="AP5" s="43"/>
-      <c r="AQ5" s="43"/>
-      <c r="AR5" s="43"/>
-      <c r="AS5" s="43"/>
-      <c r="AT5" s="43"/>
-      <c r="AU5" s="43"/>
-      <c r="AV5" s="43"/>
-      <c r="AW5" s="43"/>
-      <c r="AX5" s="43"/>
-      <c r="AY5" s="43"/>
-      <c r="AZ5" s="43"/>
-      <c r="BA5" s="43"/>
-      <c r="BB5" s="43"/>
-      <c r="BC5" s="43"/>
-      <c r="BD5" s="43"/>
-      <c r="BE5" s="43"/>
-      <c r="BF5" s="43"/>
-      <c r="BG5" s="44" t="s">
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="47"/>
+      <c r="W5" s="47"/>
+      <c r="X5" s="47"/>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="47"/>
+      <c r="AH5" s="47"/>
+      <c r="AI5" s="47"/>
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="47"/>
+      <c r="AL5" s="47"/>
+      <c r="AM5" s="47"/>
+      <c r="AN5" s="47"/>
+      <c r="AO5" s="47"/>
+      <c r="AP5" s="47"/>
+      <c r="AQ5" s="47"/>
+      <c r="AR5" s="47"/>
+      <c r="AS5" s="47"/>
+      <c r="AT5" s="47"/>
+      <c r="AU5" s="47"/>
+      <c r="AV5" s="47"/>
+      <c r="AW5" s="47"/>
+      <c r="AX5" s="47"/>
+      <c r="AY5" s="47"/>
+      <c r="AZ5" s="47"/>
+      <c r="BA5" s="47"/>
+      <c r="BB5" s="47"/>
+      <c r="BC5" s="47"/>
+      <c r="BD5" s="47"/>
+      <c r="BE5" s="47"/>
+      <c r="BF5" s="47"/>
+      <c r="BG5" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="BH5" s="44"/>
+      <c r="BH5" s="48"/>
       <c r="BI5"/>
       <c r="BJ5"/>
       <c r="BK5"/>
@@ -41670,40 +41862,40 @@
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="43"/>
-      <c r="Y5" s="43"/>
-      <c r="Z5" s="43"/>
-      <c r="AA5" s="43"/>
-      <c r="AB5" s="43"/>
-      <c r="AC5" s="43"/>
-      <c r="AD5" s="43"/>
-      <c r="AE5" s="43"/>
-      <c r="AF5" s="43"/>
-      <c r="AG5" s="43"/>
-      <c r="AH5" s="43"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="47"/>
+      <c r="W5" s="47"/>
+      <c r="X5" s="47"/>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="47"/>
+      <c r="AH5" s="47"/>
       <c r="AI5"/>
       <c r="AJ5"/>
       <c r="AK5"/>
@@ -42261,26 +42453,26 @@
       <c r="D7" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
       <c r="J7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="45" t="s">
+      <c r="K7" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
       <c r="S7" s="23" t="s">
         <v>22</v>
       </c>
@@ -42308,16 +42500,16 @@
       <c r="AA7" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="AB7" s="46" t="s">
+      <c r="AB7" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="AC7" s="46"/>
-      <c r="AD7" s="46"/>
-      <c r="AE7" s="46"/>
-      <c r="AF7" s="46"/>
-      <c r="AG7" s="46"/>
-      <c r="AH7" s="46"/>
-      <c r="AI7" s="46"/>
+      <c r="AC7" s="50"/>
+      <c r="AD7" s="50"/>
+      <c r="AE7" s="50"/>
+      <c r="AF7" s="50"/>
+      <c r="AG7" s="50"/>
+      <c r="AH7" s="50"/>
+      <c r="AI7" s="50"/>
       <c r="AJ7" s="23" t="s">
         <v>20</v>
       </c>
@@ -43112,26 +43304,26 @@
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="45" t="s">
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
       <c r="S5" s="2" t="s">
         <v>4</v>
       </c>
@@ -43558,40 +43750,40 @@
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="43"/>
-      <c r="Y5" s="43"/>
-      <c r="Z5" s="43"/>
-      <c r="AA5" s="43"/>
-      <c r="AB5" s="43"/>
-      <c r="AC5" s="43"/>
-      <c r="AD5" s="43"/>
-      <c r="AE5" s="43"/>
-      <c r="AF5" s="43"/>
-      <c r="AG5" s="43"/>
-      <c r="AH5" s="43"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="47"/>
+      <c r="W5" s="47"/>
+      <c r="X5" s="47"/>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="47"/>
+      <c r="AH5" s="47"/>
       <c r="AI5" s="35"/>
       <c r="AJ5" s="35"/>
       <c r="AK5" s="35"/>

</xml_diff>